<commit_message>
cập nhật phân công công việc
</commit_message>
<xml_diff>
--- a/Phân công công việc.xlsx
+++ b/Phân công công việc.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Xây dựng CSDL. Khung đăng nhập, menu chính</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>Học viên Lào</t>
-  </si>
-  <si>
-    <t>Xây dựng module thống kê nhân viên, viết hướng dẫn sử dụng phần mềm</t>
   </si>
 </sst>
 </file>
@@ -397,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,7 +540,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.35">
@@ -595,56 +592,23 @@
       <c r="A13" s="1">
         <v>7</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
-        <v>8</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B13:J14"/>
+  <mergeCells count="5">
     <mergeCell ref="B1:J2"/>
     <mergeCell ref="B3:J4"/>
     <mergeCell ref="B5:J6"/>

</xml_diff>